<commit_message>
feature | i-475 | Ajustes importacion masiva kits
</commit_message>
<xml_diff>
--- a/public/formats/item_sets.xlsx
+++ b/public/formats/item_sets.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BREM\Desktop\zzzzzzzzz\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4E9C203-0FAB-49DC-80EE-591F3D9D3DF9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="12330"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>Código Interno</t>
   </si>
@@ -84,12 +85,30 @@
   </si>
   <si>
     <t>CODKIT2</t>
+  </si>
+  <si>
+    <t>Descripcion</t>
+  </si>
+  <si>
+    <t>Nombre secundario</t>
+  </si>
+  <si>
+    <t>desc 1</t>
+  </si>
+  <si>
+    <t>desc 2</t>
+  </si>
+  <si>
+    <t>nombre sec 1</t>
+  </si>
+  <si>
+    <t>nombre sec 2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -401,11 +420,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -420,11 +439,11 @@
     <col min="8" max="8" width="9" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="38.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -452,8 +471,14 @@
       <c r="I1" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="J1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -481,8 +506,14 @@
       <c r="I2" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="J2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -509,6 +540,12 @@
       </c>
       <c r="I3" s="1" t="s">
         <v>17</v>
+      </c>
+      <c r="J3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K3" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feature | i-448 | Se agrega plataformas en packs/pos
</commit_message>
<xml_diff>
--- a/public/formats/item_sets.xlsx
+++ b/public/formats/item_sets.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4E9C203-0FAB-49DC-80EE-591F3D9D3DF9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BF42DBF-BB45-4D74-B5E2-F967DF367E69}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>Código Interno</t>
   </si>
@@ -103,6 +103,15 @@
   </si>
   <si>
     <t>nombre sec 2</t>
+  </si>
+  <si>
+    <t>Plataforma</t>
+  </si>
+  <si>
+    <t>Saga Falabella</t>
+  </si>
+  <si>
+    <t>Linio</t>
   </si>
 </sst>
 </file>
@@ -421,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -443,7 +452,7 @@
     <col min="12" max="12" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -477,8 +486,11 @@
       <c r="K1" t="s">
         <v>21</v>
       </c>
+      <c r="L1" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -512,8 +524,11 @@
       <c r="K2" t="s">
         <v>24</v>
       </c>
+      <c r="L2" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -546,10 +561,13 @@
       </c>
       <c r="K3" t="s">
         <v>25</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixed | i-582 | Ajustes conjuntos - pos - reportes productos - etc
</commit_message>
<xml_diff>
--- a/public/formats/item_sets.xlsx
+++ b/public/formats/item_sets.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BF42DBF-BB45-4D74-B5E2-F967DF367E69}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{447C9199-54A4-4AE4-92EA-018586E0B386}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
   <si>
     <t>Código Interno</t>
   </si>
@@ -112,6 +112,15 @@
   </si>
   <si>
     <t>Linio</t>
+  </si>
+  <si>
+    <t>Tiene Igv</t>
+  </si>
+  <si>
+    <t>SI</t>
+  </si>
+  <si>
+    <t>NO</t>
   </si>
 </sst>
 </file>
@@ -147,7 +156,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
@@ -430,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -452,7 +462,7 @@
     <col min="12" max="12" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -489,8 +499,11 @@
       <c r="L1" t="s">
         <v>26</v>
       </c>
+      <c r="M1" s="2" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -527,8 +540,11 @@
       <c r="L2" t="s">
         <v>27</v>
       </c>
+      <c r="M2" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -564,6 +580,9 @@
       </c>
       <c r="L3" s="1" t="s">
         <v>28</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed | #743 | Items Compuestos: Modelo pasa a la ultima columna
</commit_message>
<xml_diff>
--- a/public/formats/item_sets.xlsx
+++ b/public/formats/item_sets.xlsx
@@ -28,103 +28,103 @@
     <t xml:space="preserve">Código Interno</t>
   </si>
   <si>
+    <t xml:space="preserve">Código Sunat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Código Tipo de Unidad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Código Tipo de Moneda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Precio Unitario Venta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Codigo Tipo de Afectación del Igv Venta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Categoria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Descripcion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nombre secundario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plataforma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tiene Igv</t>
+  </si>
+  <si>
     <t xml:space="preserve">Modelo</t>
   </si>
   <si>
-    <t xml:space="preserve">Código Sunat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Código Tipo de Unidad</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Código Tipo de Moneda</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Precio Unitario Venta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Codigo Tipo de Afectación del Igv Venta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Categoria</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Marca</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Descripcion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nombre secundario</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Plataforma</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tiene Igv</t>
-  </si>
-  <si>
     <t xml:space="preserve">kit 1</t>
   </si>
   <si>
     <t xml:space="preserve">CODKIT1</t>
   </si>
   <si>
+    <t xml:space="preserve">NIU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PEN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bebidas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adidas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">desc 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nombre sec 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saga Falabella</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SI</t>
+  </si>
+  <si>
     <t xml:space="preserve">Modelo A</t>
   </si>
   <si>
-    <t xml:space="preserve">NIU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PEN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bebidas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adidas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">desc 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nombre sec 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Saga Falabella</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SI</t>
-  </si>
-  <si>
     <t xml:space="preserve">kit 2</t>
   </si>
   <si>
     <t xml:space="preserve">CODKIT2</t>
   </si>
   <si>
+    <t xml:space="preserve">USD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gaseosas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nike</t>
+  </si>
+  <si>
+    <t xml:space="preserve">desc 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nombre sec 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Linio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NO</t>
+  </si>
+  <si>
     <t xml:space="preserve">Modelo B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">USD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gaseosas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nike</t>
-  </si>
-  <si>
-    <t xml:space="preserve">desc 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nombre sec 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Linio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NO</t>
   </si>
 </sst>
 </file>
@@ -229,23 +229,24 @@
   <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="12.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="22.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="20"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="36.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="21.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="38.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="18.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="12.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="36.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="21.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="38.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="18.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="12.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="12.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -270,13 +271,13 @@
       <c r="G1" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="0" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="0" t="s">
@@ -285,10 +286,10 @@
       <c r="L1" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="0" t="s">
         <v>13</v>
       </c>
     </row>
@@ -299,28 +300,28 @@
       <c r="B2" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="0" t="n">
+        <v>20202020</v>
+      </c>
+      <c r="D2" s="0" t="s">
         <v>16</v>
-      </c>
-      <c r="D2" s="0" t="n">
-        <v>20202020</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="F2" s="0" t="n">
+        <v>120.25</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="G2" s="0" t="n">
-        <v>120.25</v>
-      </c>
-      <c r="H2" s="0" t="n">
-        <v>10</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" s="0" t="s">
         <v>20</v>
       </c>
       <c r="K2" s="0" t="s">
@@ -329,10 +330,10 @@
       <c r="L2" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="M2" s="0" t="s">
+      <c r="M2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="N2" s="0" t="s">
         <v>24</v>
       </c>
     </row>
@@ -343,40 +344,40 @@
       <c r="B3" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="0" t="n">
+        <v>51121703</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="0" t="n">
-        <v>51121703</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="0" t="s">
+      <c r="F3" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="G3" s="0" t="n">
-        <v>150</v>
-      </c>
-      <c r="H3" s="0" t="n">
-        <v>10</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J3" s="0" t="s">
         <v>30</v>
       </c>
       <c r="K3" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="L3" s="0" t="s">
+      <c r="L3" s="1" t="s">
         <v>32</v>
       </c>
       <c r="M3" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="N3" s="0" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>